<commit_message>
Update QA Documentation. Close #12
</commit_message>
<xml_diff>
--- a/Documents/Task_Schedule-QA.xlsx
+++ b/Documents/Task_Schedule-QA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\source\repos\Fire-Department-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292BF47E-1B30-46D6-81E7-DE20501C2008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45E0807-39A2-4D1D-84B3-070EFF1AD319}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Deadline</t>
   </si>
@@ -105,36 +105,9 @@
     <t>26.04.2021</t>
   </si>
   <si>
-    <t>26.04.2022</t>
-  </si>
-  <si>
-    <t>26.04.2023</t>
-  </si>
-  <si>
-    <t>26.04.2024</t>
-  </si>
-  <si>
-    <t>26.04.2025</t>
-  </si>
-  <si>
-    <t>26.04.2026</t>
-  </si>
-  <si>
-    <t>26.04.2027</t>
-  </si>
-  <si>
-    <t>26.04.2028</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>19.04.2021</t>
   </si>
   <si>
-    <t>18.04.2022</t>
-  </si>
-  <si>
     <t>06.04.2021</t>
   </si>
   <si>
@@ -142,13 +115,19 @@
   </si>
   <si>
     <t>09.04.2021</t>
+  </si>
+  <si>
+    <t>22.04.2021</t>
+  </si>
+  <si>
+    <t>25.04.2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +148,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,14 +165,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC5C5"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -251,8 +230,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -260,8 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,8 +249,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,7 +541,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,15 +556,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -621,13 +602,13 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -644,13 +625,13 @@
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>37</v>
+      <c r="E4" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -665,15 +646,15 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -690,13 +671,13 @@
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -713,13 +694,13 @@
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -734,14 +715,16 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -757,12 +740,14 @@
       <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,14 +761,16 @@
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>